<commit_message>
Added RoBERTa, Longformer. Combined results into a single data frame to compare them.
</commit_message>
<xml_diff>
--- a/src/data/sentiment_results/sentiment_results_BERT_large.xlsx
+++ b/src/data/sentiment_results/sentiment_results_BERT_large.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="57">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -34,7 +34,10 @@
     <t>Stock_Value</t>
   </si>
   <si>
-    <t>Predicted_Sentiment</t>
+    <t>Row_Number</t>
+  </si>
+  <si>
+    <t>BERT_Large_Sentiment</t>
   </si>
   <si>
     <t>Heidelberg Materials</t>
@@ -58,9 +61,6 @@
     <t>Siemens Energy</t>
   </si>
   <si>
-    <t>Adidas</t>
-  </si>
-  <si>
     <t>News</t>
   </si>
   <si>
@@ -106,12 +106,6 @@
     <t>2021-06-22</t>
   </si>
   <si>
-    <t>2021-06-24</t>
-  </si>
-  <si>
-    <t>2021-06-25</t>
-  </si>
-  <si>
     <t>Heidelbergcement klimaneutral Zementwerk Weg Biontech Impfstoff Belgien Handelsstreit keimt zart Pflänzchen USA China Hintergrund andauernd handelsstreit China Vizepremier Liu neu Usfinanzministerin janet Yellen Videogespräch austauschen laut Erklärung chinesisch Handelsministerium Gespräch Mittwoch Frage beiderseitig Interesse diskutieren Detail Staat formell Verhandlung Beilegung zollkriegs beginnen erstmals Amtsübernahme neu Uspräsident Joe bid Unterhändler USA China andauernd Handelskrieg vergangen Woche miteinander Kontakt aufnehmen neu ushandelsbeauftragt Katherine Tai ebenfalls liu austauschen Peking Handelsfrag zuständig neu Regierung Joe bid begreifen China Konkurrent andeuten ebenfalls hart Kurs Peking verfolgen Abstimmung international verbündeter China unfair Handelspraktike unangemessen staatlich Subvention marktbarrieren Diebstahl geistig Eigentum zwangsweis Technologietransfer vorwerfen Dax Tag Dax Mittwoch moderat Kursgewinn Nähe Vortag erreicht Rekordhoch halten Minute Eröffnung verbuchen Leitindex Plus Prozent Punkt Dienstag Zähler zulegen früh Nachmittag Teil Gewinn abgeben Wall Street Stärke europäisch Börse aufnehmen marktexpert fragen Kursniveau Anleger gewinnmitnahmen verleiten Käufe animiert Mdax mittelgroß deutsch Unternehmen gelingen Mittwoch Rekord zuletzt notieren plus Prozent Punkt Eurozonenleitindex Eurostoxx rücken Prozent Heidelbergcement klimaneutral Zementwerk Welt daxkonzern bestehend Anlage slit Schwede Insel Gotland ausbauen jährlich Million Tonne Kohlendioxid abgeschieden entsprechen gesamt Emission Werk teilen Unternehmen Mittwoch co2 dauerhaft Lagerstätte mehrere Kilometer Tiefe Grundgestein Meer transportieren Branche Vorreiter Weg co2neutralität sagen Konzernchef Dominik Nachrichtenagentur Reuters Heidelbergcement zweitgrößter Hersteller energieintensiv produziert Baustoff Zement Lafargeholcim Weltmarktführer Schweiz liefern deutsch Unternehmen Druck Klimapolitik Investor Wettstreit Abbau treibhausgasen wichtig Dekarbonisierung Ziel formulieren konkret Projekt umsetzen schnell betonen Konzernchef bestehend Werk Slit laut Heidelbergcement derzeit Viertel Betonproduktion Schweden verwendet Zements herstellen Umbau Werk sprechen dreistellig Millionenbetrag sagen Heidelbergcement bereit Anteil tragen überwiegend Teil Kosten schwedisch Regierung übernehmen Projekt unterstützen ehrgeizig Ziel Schweden Reduzierung co2emissione Ausbau Slit Heidelberger norwegisch Werk Brevik gewonnen Erfahrung profitieren bauen Konzern Angabe weltweit großtechnisch Anlage co2abscheidung jährlich Tonne beziehungsweise Prozent Emission Werk abschieden Biontechpfizer Impfstoff Belgien erfolgreich paar Pharmabranche Werk belgisch Puurs Produktion Coronaimpfstoff hochfahren europäisch Arzneimittelbehörde Ema empfehlen Dienstag Herstellung Abfüllungskapazität genehmig erheblich sofortig Auswirkung Versorgung Impfstoff Mainzer Firma Biontech uspartn Pfizer erklären Ema Biontechpfizer bestätigen Anfrage Impfstoffkapazität ausweiten Emaempfehlung Bemühung unterstützen laufend Jahr Milliarde dosen Impfstoff ausliefern nächster Jahr möglicherweise ema stellen Prüfung fest Fabrik Puurs durchgängig Impfstoff Qualität produzieren ermöglichen Biontechpfizer Menge hergestellt Impfstoff steigern Eugesundheitskommissarin stella Kyriakide begrüßen Twitter willkommen Schritt Erhöhung Produktionskapazität europäisch Union schneller Lieferung impfstoffen Welt Curevac fleißig daten sammeln Monat Impfstoff Konkurrenz verabreichen Zulassung Vakzin Tübinger Biotechunternehmen Curevac daten sammeln Juni vorliegen Sprecher Dienstag bekräftigen ermöglichen rollierend Zulassungsverfahr europäisch Arzneimittelagentur Ema finalisieren zuvor mehrere Medium berichten unabhängig Data safety monitoring Board Dsmb sehen Sicherheitsbedenke Impfstoff Cvncov teilen Sprecher zudem bestätigen Studie fortsetzen ausreichend Anzahl daten Durchführung statistisch signifikant wirksamkeitsanalyse sammeln Zwischenanalyse Bestätigung Fortschritt Studie normal Prozedere erläutern Sprecher Notwendigkeit erhöht statistisch Aussagekraft angesichts komplex klinisch Studiendate ungewöhnlich bedeuten Impfstoff möglicherweise wirksam bedeuten daten benötigen fundiert Berechnung Impfstoffwirksamkeit ermöglichen Unternehmen Zugang anonymisiert Studiendate Dsmb Fortgang Studie informieren knapp auto1 verschieden Aktionär Onlinegebrauchtwagenhändler laut kreisen insgesamt knapp million Aktie Profiinvestor platzieren entsprechen Prozent Aktie Sdax notiert Unternehmen Angebot mehrere Beteiligungsgesellschaft richten beschleunigt Preisbildungsverfahr institutionell Investor heißen dienstagabend Börsenschluss Nachrichtenagentur Bloomberg eingesehen angebotsunterlag berufen Auto1 Börse insgesamt zuletzt Milliarde Euro bewerten Gründer Christian Bertermann Hakan Koç halten knapp Prozent Anteil folgen japanisch Technologieinvestor Mischkonzern Softbank zuletzt Prozent Volvo schwedisch nutzfahrzeughersteller verkaufserlös Lkwbauer Trucks Aktionär weiterreich Anfang April Schwede Verkauf Marke Milliarde schwedisch Krone mrd Euro Isuzu Motors abschließen Ende Juni außerordentlich Aktionärsversammlung Ausschüttung Geld billigen Dienstag Volvo Stockholm heißen pro Aktie Krone Aussicht stellen Abschluss Deal Quartal positiv Effekt Milliarde Krone operativ Ergebnis Folge Volvo Abschluss mitteilen Jbs Hackerangriff weltgrößter Fleischkonzer Brasilien Teil Produktion Nordamerika Australien lahmlegen Sprecherin weiß Haus erklären Dienstag Ortszeit Washington Jbs Usregierung Sonntag Attacke informieren zuvor brasilianisch Unternehmen Tochter Jbs USA mitteilen Ziel organisiert Cyberattacke Angriff Server Itsystem Nordamerika Australien treffen Zeit dauern Problem beheben Detail nennen Jbs Angabe Usregierung fordern Hacker Lösegeld Jbs weiß Haus Kenntnis setzen Forderung kriminell Organisation stammen vermutlich Russland Regierung Russland klarmachen verantwortungsvoll Staat Urheber Attacke beherberge Usbundespolizei Fbi einschalten ermittlen Redaktion Onvista dpaafx Reuters Foto Homepage Heidelbergcement basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
   </si>
   <si>
@@ -175,18 +169,6 @@
     <t>Microsoft Softwaregigant Knackt Marktkapitalisierung Billion Dollar Gamestop Aktienverkäufe spülen milliarde Dollar Kasse Vonovia Übernahmeangebot starten Jerome Powell zumindest amerikanisch Anleger beruhigen Aussage Fedchef Unterausschuss Repräsentantenhaus Teuerung vorübergehend Natur sobald engpässe Angebotsseite abschwächten Inflation zurückgehen bekräftigen Einschätzung beruhigen zuletzt nervös Investor Usakti daraufhin zulegen Technologiebörse nasdaq melden Rekordhochs indiz wichtig Powell Fahrplan kommend Monat präsentieren obwohl Entscheidungsgremium amerikanisch Notenbank Stimme Drosselung Anleihenkauf geben Punkt Neuigkeit Anleger zusätzlich beruhigen Vorgabe USA nehmen Dax früh bedingt dax Powell beruhigen bedingt beruhigend Wort jerome Powell Sache Inflation Kurse deutsch Aktienmarkt Mittwoch helfen Leitindex Dax rücken Handelsminut Prozent Punkt vorbei grün Vorzeichen mittlerweile deutsch Leitindex Vortagsniveau abgerutscht Mdax mittelgroß Börsentitel Prozent Zähler Eurostoxx Leitindex Eurozone zeigen fest Microsoft Billion Dollar börsenwern Softwaregigant Börse erstmals Billion Dollar Wert Papier profitieren Dienstag allgemein Markterholung schwach vorwoch steigen Handelsschluss Favorit Dow Jones Industrial Prozent Usdollar Usleitindex rücken Ende Prozent Microsoft Computerkonzern Apple Usaktiengesellschaft Marktkapitalisierung Billion Dollar aufweisen Rangliste wertvollst Börsennotiert uskonzerne halten Apple aktuell Platz Billion Dollar Onlinehändler Amazon Googlemutter Alphabet liegen Microsoft Plätz folgen Onlinenetzwerk Facebook Beteiligungsgesellschaft Berkshire Hathaway elektroautobauer Tesla Jahresbeginn Aktie Microsoft Prozent zulegen Anleger wetten derzeit Dominanz Unternehmen Geschäft mietsoftware Internet Cloud Gebiet unternehmenssoftwar Coronakrise sogar zunehmen Dienstag stützen positiv Analystenkommentar Kurs möglicherweise Microsoft Donnerstag anstehend Veranstaltung neu Betriebssystem windows vorstellen schreiben Experte Karl Keirstead schweizerisch Großbank ubs Interesse Software potenziell Einführung Abolizenzmodell Bewertung Microsoftaktie erscheinen aktuell Niveau rechtfertigen Gamestopp Milliarde Dollar frisch Kasse Usvideospielhändler Gamestop außergewöhnlich Kursrally Schlagzeile bringen Milliarde Dollar Aktienverkauf einnehmen kriselnd Unternehmen profitieren Kampagne Internet organisiert Kleinanleger Jahresbeginn Aktienpreis steigen lassen Gamestop verkaufen vergangen Woche Million Anteilsschein insgesamt knapp Milliarde Dollar Mio Euro Geld wachstumsinitiativ Stärkung Bilanz verwenden Unternehmen Dienstag mitteilen Aktie kosten Anfang Januar Dollar steigen binnen Woche Spitze knapp Dollar bevor Talfahrt einsetzen früh Ushandel Dienstag legen Kurs Ankündigung Prozent Dollar Gamestop stecken läden eigentlich Krise eröffnen Kursaufschwung Unternehmen neu Möglichkeit Firma angestaubt Geschäftsmodell klassisch Einzelhandelskette verabschieden modern Technologieanbieter Onlinegamer geschäftlich laufen Gamestop zuletzt Monat Anfang Mai steigen Umsatz jahresvergleich Viertel Milliarde Dollar Gamestop schreiben rot Zahl verringern Verlust binnen Jahr Million Dollar Bitcoins kaufen erfahren erfolgreich Kryptowährung worauf Bitcoin Traden ankommen knapp Vonovia Deutschland Immobilienkonzer beginnen geplant Übernahme deutsch wohnen Aktionär Konkurrent Juli Mitternacht Zeit Offerte annehmen Vonovia Mittwoch Bochum mitteilen Vonovia Ende Mai deutsch wohnen Übernahme Konzern bieten Aktionär deutsch wohnen pro Aktie Euro bar Shop Apotheke bankhaus Metzler Shop Apotheke buy Hold abstufen Kursziel Euro senken Einführung elektronisch Rezept holprig verlaufen erwarten schreiben Analyst Tom diedrich Mittwoch vorliegend Studie zurückliegend Monat Aktie schlagen Konkurrenz Spielraum begrenzen tui Touristikkonzernsieht Konzerneigene Flugzeugflotte Sparbeschlüsse coronaeinbrüchen rüsten lässt Thema Staatshilfenrückzahlung Zeit weltgrößter Reiseanbieter Sommer Geld einnehmen belastbar sagen Finanzchef Sebastian Ebel nachrichtenagenturen dpa Dpaafx Teil steuerfinanziert Milliardenkredite zurückfließen derzeit genau absehen bike24 Onlinefahrradspezialist letzter Hürde Weg Börsengang nehmen Preis angeboten Aktie Euro Papier festlegen teilen Fahrräder Fahrradzubehör Bekleidung spezialisiert Unternehmen dienstagabend Dresden unterer Ende zuvor angegeben Preisspanne erreichen Euro liegen insgesamt Million Aktie institutionell Investor platzieren heißen stammen Million hauptsächlich Bestand aktuell Mehrheitseigentümer europäisch Riverside Fonds verbunden Gesellschaft Gesamtbruttoerlös Höhe Million Euro erhalten Bike24 Million Euro Drittel Geld Unternehmen Angabe zufolge Beschleunigung international Wachstum stecken anfänglich Marktkapitalisierung liegen Million Euro Handelstag reguliert Markt Prime Standard Frankfurter Wertpapierbörse Juni Krispy kreme Firmenimperium deutsch Milliardärsfamilie Reimann gehörend Usdonutkette hoffen Einnahme Million Dollar anstehend Börsengang oberer Ende Preisspanne Dollar pro Aktie Bewertung Krispy Kreme Richtung Marke Milliarde Dollar aktualisiert Börsenprospekt Dienstag hervorgehen Anteilsscheine Börse nasdaq kürzel dnut notieren Reimanninvestmentholding Jab Krispy Krem Milliarde Dollar kaufen Börse nehmen Kette verkaufen vergangen Geschäftsjahr Milliarde Donuts setzen inzwischen stark Onlinehandel Familie Börsengang klar Mehrheit knapp Prozent Anteil behalten Jabholding gehören anderer Gastronomiekett Pret Manger Panera Bread Redaktion Onvista dpaafx Foto Jeanlucichard Shutterstockcom basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
   </si>
   <si>
-    <t>deutsch Bank Sap Google packen Oracle itsystemen Sparpotenzial Milliardenhöhe Zusammenführung verschieden Itsystem Frankfurter Baustelle Microsoft deutsch Bank Uskonzer Boot holen Itabteilung Vordermann bringen Hilfe softwareriesen Oracle erneuern Christian Sewing Itsystem Finanzinstitut erneuern Cloud Oracle mehrere Datenbank kritisch Bereich zahlungsverkehr Handel Kapital Risikosteuerung Plattform privat Cloud übertragen erklären Konzern Donnerstag deutsch Bank kommend Jahr niedrig dreistellig Millionenbetrag einsparen sagen Technologiechef Bernd Leukert Nachrichtenagentur Reuters Bank Dienstleistung oracle zahlen erläutern Jahr leukert zahlreich neu Itfachkräft einstellen einfach strategisch Partnerschaft Oracle Komplexität Itlandschaft verringern sagen Leukert Ziel Bank Drittel System betreiben Jahr Migration abschließen finanziell Vorteil schnell realisieren gesamt Kosten Bank zuletzt Milliarde Euro Milliarde Euro sinken System deutsch geldhauses gelten Jahr Marode fehleranfällig Exbankchef John Cryan öffentlich lausig bezeichnen ehemalig Sapvorstand Leukert deutsch Bank stellen Itlandschaft komplett neu setzen personell Ausbau Itteam alleine Jahr Zahl Job Bereich brutto steigen kündigen Leukert Veranstaltung Börsenzeitung Ziel Ende Hälfte Mitarbeiter Bereich Technologie daten Innovation Softwareingenieure beschäftigt Ende Anteil Prozent liegen Oracle kümmern zusammenführung Plattformen privat Cloud Rechenzentren deutsch Bank betreiben erklären Institut Migration ermöglichen Ablauf standardisieren Anwendung skalieren Nutzung privat Cloud kritisch daten schützen öffentlich Datenwolke Finanzaufsicht verlangen Bank Itdienstleister bestimmt daten umfangreich Schutzmechanismen potenziell Hackerangriffe oracle betreiben ähnlich privat Cloudangebote zahlreich anderer Bank Projekt deutsch Bank bislang sagen Oraclemanager Juan Loaiza Datenbanken kritisch Information zuständig kritisch Anwendung nutzen Frankfurter Geldhaus Couldangebote Google Partnerschaft Kooperation Oracle ergänzen sagen Leukert Walldorfer softwarekonzern Sap weiterhin zusammengearbeitet Redaktion Onvista Reuters Foto 1take1shotshutterstockcom basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
-  </si>
-  <si>
-    <t>adidas stark Nikezahlen beflügeln Konkurrenz deutsch Post Fedexzahlen ziehen Aktie runter Hornbach stark Ausblick Dax fast unverändert Vortageskurs Handel starten vorbörslich Handel gewinne abzeichnen Punkt notieren Handelsbeginn Prozent plus Dax bisweilen stehaufmännch vorkommen kommentieren Experte Helaba einerseits zeigen geraum Zeit Spielraum oberseite ausreizen scheinen andererseits zwischenzeitlich Rücksetzer zügig aufholen heißen Kommentar Landesbank Modus bewegen vergangen Tag Punkt Leitindex folgen usbörsen eher gedrosselt Tempo Wall Street Technologieindize Nasdaq marktbreit neu höchstständ Nase voraus Dax rücken Rekord Punkt Montag Woche alt nah ankleangen Anleger finden Fortschritt uspräsident Joe biden ringen billionenschw Investition Infrastruktur trotz Deal Zustimmung Kongress gewiss verkünden Uspräsident Einigung klein Gruppe demokratisch republikanisch Senator Paket Investition Straße brücken Verkehrs energienetze erhalten Usbank Rahmen Stresstest positiv Feedback Usnotenbank heben Einschränkung Aktienrückkäufe Dividende Freitag hierzulande Sektorwert ankommen Aktie deutsch Bank vorbörslich Prozent stark Nikezahle pushen adidas Anstieg Prozent vorbörslich Adidaspapier Blick Wert verweisen Börsianer Kurssprung Prozent Anteil Wettbewerbers Nike nachbörslich Ushandel Ussportartikelhersteller übertreffen Zahl vergangen Quartal Markterwartung deutlich neu jahresprognos überzeugen Börsianer Umsatz Milliarde Dollar fast doppelt Jahr zuvor Analyst Ende Mai abgeschlossen Geschäftsquartal eher erlösen Milliarde Dollar rechnen Strich verdienen Nike Milliarde Dollar Verlust Million Dollar Vorjahresquartal Adidasrivale Usbörsenschluss Donnerstag mitteilen Gewinn pro Aktie erreichen Uscent Analyst Cent ausgehen Haar Suppe dennoch finden umsätze Amerikaner China denken wofür Reaktion Chinesen Sanktion Zusammenhang Region xinjiang Minderheit uiguren verantwortlich Analyst reagieren positiv Puma stocken Experte kursziele signalisieren deutlich Potenzial deutsch Post Fedexzahl Druck setzen Verliererseite stehen vorbörslich zuletzt rekordhohe Aktie deutsch Post Plattform Tradegate halb Prozent fallen blicken Uswettbewerber richten Fedex verfehlen Ausblick Erwartung Aktie Logistiker nachbörslich Ushandel Prozent Druck geraten Fedex vorgelegt Zahl Geschäftsquartal geben positiv Feedback Belastung empfanden Händler Ausblick neu Geschäftsjahr Börsianer betonen verfehl Erwartung lohnkosten niedrig gedacht Produktivität Fedex schränken Prognose anstehend Bilanzielle Anpassunge Pensionsplän weiterhin genau beziffern Hornbach punkten stark Ausblick Aktie Hornbach Blick wert Papier Freitag vorbörslich quartalsbericht antreiben Handelsplattform Tradegate rücken Titel vergleichen xetraschlusskurs Prozent Reaktion heißen Markt Ausblick Baumarktholding Anleger ankommen Händler zufolge überzeugen erwartet Zahlenwerk Geschäftsquartal ebenfalls börsennotiert Aktie Tochter Hornbach Baumarkt vorbörslich sogar fast Prozent beflügeln anhaltend Nachfrage steigen Quartalserlös Konzernweit Prozent Milliarde Euro Konzern äußern Basis laufend Geschäftsjahr optimistisch rechnen Vorstand Erlösplus bislang Umsatz Vorjahresniveau ausgehen operativ Ergebnisziel bereinigt Ebit präzis formulieren Million Euro liegen Onvistadpaafx Titelfoto bjoern wylezich Shutterstockcom Onvistaratgeber kostenlos Girokonto Thema girokontovergleich basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
-  </si>
-  <si>
-    <t>glänzend Zahl Nike treiben Aktienkurs Erwartung adidas Puma Höhe nike gestern spät Ushandel glänzend quartalszahl Punkt kräftig Gewinn Börse verzeichnen hiesig Konkurrenz arm greifen Papier Adidas Puma ziehen Adidas steigen Daxspitze Prozent Stand Anfang Puma fallen Aufschlag knapp Prozent knapp Kurs erklomm dennoch Rekordhoch überwehen erstmals 100euromark Nike Rekordhoch spät Usaktiengeschäft nike sogar Prozent schießen Rekordhoch Sportartikel Lifestylekonzer profitieren kräftig Aufhebung coronabeschränkunge USA Umsatz Nordamerika schoss vergangen Quartal Prozent knapp Milliarde Dollar weltweit Erlös Milliarde Dollar mrd Euro fast doppelt Jahr zuvor Strich verdienen Unternehmen Monat Milliarde Dollar adidas Puma folgen Nachfrage märkten Nordamerika Europa quasi Bühne frei ähnlich erfreulich Quartalsberichte Adidas Puma kommend Woche kommentiert Analyst James Grzinic Usbank Jefferies betitelen Analyse crikey Nike deutsch Güte nike Umsatz Monat März Mai liegen Prozent Markterwartung enorm aufholen Großhandel geschäftsquartal Auslieferung verzögern Übertragung Wachstumsrate Nike Adidas Puma schwierig schränkt Grzinic gegenwärtig Konsensschätzung deutsch Kontrahent liegen Nike Vorabend gemeldet werten gelten adidas Puma gleichwohl belegen abschneiden Nike weltweit stark steigend Nachfrage adidas Puma profitieren angesichts nachfragebooms Adidaskurs knapp Euro neu Kaufempfehlung Papier ausrufen Analyst raten derzeit knapp Hälfte halten Aktie Lage Puma empfehlen Fachleut Kauf Aktie Aufwärtspotenzial Kursziele belaufen Euro sodass Anteilschein nurmehr Prozent Aufwärtspotenzial einräumen Onvistadpaafx Titelfoto 2p2play Shutterstockcom Onvistaratgeber ökofonds finden nachhaltig Geldanlagen basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
-  </si>
-  <si>
-    <t>Dax Leitindex retten plus Wochenende Adidas sprinten Höhe Hornbach legen Schippe drauf korrigieren dax De0008469008 Wochenende Luft ausgehen mangels impuls schloss deutsch Leitindex Freitag Prozent plus Punkt stark Schwankung geprägt Börsenwoche stehen Gewinn Prozent buchen Angriff Rekordhoch Zähler reichen zuletzt Mdax De0008467416 mittelgroße Börsenwert schlagen legen Prozent Zähler einerseits zeigen geraum Zeit Spielraum oberseite ausreizen scheinen andererseits zwischenzeitlich Rücksetzer zügig aufholen schreiben Analyst Christian Schmidt Landesbank Helaba Dax erweise stehaufmännch zumal Trend Mittel langfristig aufwärts weisen Lage bleiben spannend kursen Punkt drohen Verkaufsdruck Anstieg Prozent setzen Aktie adidas de000a1ewww0 klar daxspitz Grund stark Umsatzsprung Wettbewerber Nike us6541061031 Aktie New York Prozent schnelln Adidastitel schaffen Spitze Euro Anfang Puma profitieren stark Zahl nike erklommen Rekordhoch Euro schließen Prozent Verliererseite stehen zuletzt rekordhohe Aktie deutsch Post de0005552004 Prozent sinken blicken Uswettbewerber richten Fedex Us31428x1063 verfehlen Ausblick Erwartung fragen Aktie Bausektor profitieren Fortschritt uspräsident Joe biden ringen billionenschw Investition Infrastruktur bid verkünden Donnerstag Einigung Gruppe demokratisch republikanisch Senator Paket Investition Verkehrs energienetze Aktie Heidelbergcement de0006047004 rücken Prozent Baudienstleister hochtief De0006070006 Mdax Prozent Dax Schwung Eli Lilly Adidas Warren buffett attraktiv Übernahmeziel finden     Folge verpassen einfach Onvista Youtubekanal abonnieren Nachricht Tag Frage bernecker geldpolitisch Sackgasse attraktiv Air Liquide Curevac herantrauen Aktie spekulativ Rally Korrekturmodus ipo chinesisch Uberrivale Didi Chuxing streben Börse Softbank Anteilseigner glänzend Zahl Nike treiben Aktienkurs Erwartung adidas Puma Höhe Bitcoin Salvador Einwohner Bitcoin Wert Dollar zukommen lassen überraschend stark geschäftsquartal attestiert Analyst Baumarktkonzer Hornbach Papier Hornbach Holding De0006083405 schießen fast Prozent Unternehmen laufend Geschäftsjahr optimistisch Anleger Begeisterung sorgen Druck stehen Aktie de000ksag888 Prozent Abrutscht nehmen Anleger Kursgewinn Kurs Mitte April Mitte Juni Zug steigend Kalipreise Hälfte steigen beschäftigen Freitag Börsengang Anleger Aktie Bike24 de000a3cq7f4 Onlineversandhändler Fahrräder Zubehör beenden Börsentag Euro ausgeben Unternehmen Aktie Euro unterer Rand Angebotsspanne europäisch Börse zeigen überwiegend bewegen Eurostoxx Eu0009658145 schloss Prozent niedrig Punkt Pariser Cac Index geben ebenfalls moderat Londoner Ftse Drittelprozent zulegen USA stehen Dow Jones Industrial Us2605661048 europäisch Handelsschluss Prozent Vortagesniveau Euro eu0009652759 zuletzt Usdollar handeln europäisch Zentralbank Referenzkurs Nachmittag Dollar festsetzen Umlaufrendite deutsch Bundesanleihen sinken Freitag minus Prozent minus Prozent Rentenindex rex De0008469107 legen Prozent Punkt Bundfutur de0009652644 geben Abend Prozent Punkt Benjamin Krieger Dpaafx Foto Anathomy Shutterstockcom basisprospekt endgültig Bedingung Basisinformationsblätter erhalten Klick Dokumentensymbol beachten Hinweis Werbung</t>
-  </si>
-  <si>
     <t>positive</t>
   </si>
   <si>
@@ -202,7 +184,7 @@
     <t>neutral</t>
   </si>
   <si>
-    <t>Neutral</t>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -560,13 +542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,10 +570,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -603,18 +588,21 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -626,18 +614,21 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>52</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -649,18 +640,21 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>53</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -672,18 +666,21 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>54</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -695,18 +692,21 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>54</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -718,18 +718,21 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -741,18 +744,21 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -764,18 +770,21 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -787,18 +796,21 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>53</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -810,18 +822,21 @@
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -833,18 +848,21 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>54</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -856,18 +874,21 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -879,18 +900,21 @@
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -902,18 +926,21 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -925,18 +952,21 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -948,18 +978,21 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -971,18 +1004,21 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>54</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -994,18 +1030,21 @@
         <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>53</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -1017,18 +1056,21 @@
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -1040,18 +1082,21 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>52</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -1063,105 +1108,16 @@
         <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>